<commit_message>
Added new files. Also Updated text document.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitTrial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\FirstTestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9796A3EF-2996-4495-A223-222510E73C6B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47226D09-901E-4883-9F46-5F49E30E7D61}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{71FAC163-608D-4B58-BEFB-E4048A150304}"/>
   </bookViews>
@@ -371,12 +371,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B787BAF-D049-441F-961E-3B812CA412B7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>